<commit_message>
Finalized to 5 ideas
</commit_message>
<xml_diff>
--- a/Divide and Conquer results.xlsx
+++ b/Divide and Conquer results.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="41 to 20" sheetId="1" r:id="rId1"/>
-    <sheet name="20 to 10" sheetId="2" r:id="rId2"/>
+    <sheet name="20 to 5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -92,15 +92,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <f>AVERAGE(B2,C2,D2,E2)</f>
+        <f t="shared" ref="F2:F42" si="0">AVERAGE(B2,C2,D2,E2)</f>
         <v>4.75</v>
       </c>
     </row>
@@ -473,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="2">
-        <f>AVERAGE(B3,C3,D3,E3)</f>
+        <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
     </row>
@@ -494,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="2">
-        <f>AVERAGE(B4,C4,D4,E4)</f>
+        <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
     </row>
@@ -515,7 +516,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="2">
-        <f>AVERAGE(B5,C5,D5,E5)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -536,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <f>AVERAGE(B6,C6,D6,E6)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -557,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="2">
-        <f>AVERAGE(B7,C7,D7,E7)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -578,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="2">
-        <f>AVERAGE(B8,C8,D8,E8)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -599,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="2">
-        <f>AVERAGE(B9,C9,D9,E9)</f>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
     </row>
@@ -620,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="2">
-        <f>AVERAGE(B10,C10,D10,E10)</f>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
     </row>
@@ -641,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="2">
-        <f>AVERAGE(B11,C11,D11,E11)</f>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
     </row>
@@ -662,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2">
-        <f>AVERAGE(B12,C12,D12,E12)</f>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
     </row>
@@ -683,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="2">
-        <f>AVERAGE(B13,C13,D13,E13)</f>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
     </row>
@@ -704,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="2">
-        <f>AVERAGE(B14,C14,D14,E14)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -725,7 +726,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="2">
-        <f>AVERAGE(B15,C15,D15,E15)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -746,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="2">
-        <f>AVERAGE(B16,C16,D16,E16)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -767,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="2">
-        <f>AVERAGE(B17,C17,D17,E17)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -788,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="2">
-        <f>AVERAGE(B18,C18,D18,E18)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
@@ -809,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="2">
-        <f>AVERAGE(B19,C19,D19,E19)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
@@ -830,7 +831,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="2">
-        <f>AVERAGE(B20,C20,D20,E20)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
@@ -851,7 +852,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="2">
-        <f>AVERAGE(B21,C21,D21,E21)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
@@ -872,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="4">
-        <f>AVERAGE(B22,C22,D22,E22)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -893,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="4">
-        <f>AVERAGE(B23,C23,D23,E23)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -914,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="4">
-        <f>AVERAGE(B24,C24,D24,E24)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -935,7 +936,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="4">
-        <f>AVERAGE(B25,C25,D25,E25)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -956,7 +957,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="4">
-        <f>AVERAGE(B26,C26,D26,E26)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -977,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="4">
-        <f>AVERAGE(B27,C27,D27,E27)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -998,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="4">
-        <f>AVERAGE(B28,C28,D28,E28)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -1019,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="4">
-        <f>AVERAGE(B29,C29,D29,E29)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -1040,7 +1041,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="4">
-        <f>AVERAGE(B30,C30,D30,E30)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -1061,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="4">
-        <f>AVERAGE(B31,C31,D31,E31)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -1082,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="4">
-        <f>AVERAGE(B32,C32,D32,E32)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -1103,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="4">
-        <f>AVERAGE(B33,C33,D33,E33)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1124,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="4">
-        <f>AVERAGE(B34,C34,D34,E34)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1145,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="4">
-        <f>AVERAGE(B35,C35,D35,E35)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1166,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="4">
-        <f>AVERAGE(B36,C36,D36,E36)</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -1187,7 +1188,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="4">
-        <f>AVERAGE(B37,C37,D37,E37)</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -1208,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="4">
-        <f>AVERAGE(B38,C38,D38,E38)</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -1229,7 +1230,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="4">
-        <f>AVERAGE(B39,C39,D39,E39)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1250,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="4">
-        <f>AVERAGE(B40,C40,D40,E40)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1271,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="4">
-        <f>AVERAGE(B41,C41,D41,E41)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
     </row>
@@ -1292,7 +1293,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="4">
-        <f>AVERAGE(B42,C42,D42,E42)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
     </row>
@@ -1310,11 +1311,12 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -1337,7 +1339,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3">
         <v>5</v>
@@ -1346,585 +1348,746 @@
         <v>5</v>
       </c>
       <c r="D2" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2">
         <f>AVERAGE(B2,C2,D2,E2)</f>
-        <v>4</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2">
+        <v>4.75</v>
+      </c>
+      <c r="G2" s="7">
+        <v>5</v>
+      </c>
+      <c r="H2" s="7">
+        <v>5</v>
+      </c>
+      <c r="I2" s="7">
+        <v>5</v>
+      </c>
+      <c r="J2" s="7">
+        <v>4</v>
+      </c>
+      <c r="K2" s="3">
         <f>AVERAGE(G2,H2,I2,J2,F2)</f>
-        <v>4</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
       </c>
       <c r="C3" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <f>AVERAGE(B3,C3,D3,E3)</f>
-        <v>3.5</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3">
-        <f t="shared" ref="K3:K20" si="0">AVERAGE(G3,H3,I3,J3,F3)</f>
-        <v>3.5</v>
+        <v>4.25</v>
+      </c>
+      <c r="G3" s="7">
+        <v>5</v>
+      </c>
+      <c r="H3" s="7">
+        <v>5</v>
+      </c>
+      <c r="I3" s="7">
+        <v>4</v>
+      </c>
+      <c r="J3" s="7">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3">
+        <f>AVERAGE(G3,H3,I3,J3,F3)</f>
+        <v>4.25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3">
         <v>4</v>
       </c>
       <c r="E4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2">
         <f>AVERAGE(B4,C4,D4,E4)</f>
-        <v>3.5</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>4.25</v>
+      </c>
+      <c r="G4" s="7">
+        <v>5</v>
+      </c>
+      <c r="H4" s="7">
+        <v>5</v>
+      </c>
+      <c r="I4" s="7">
+        <v>4</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <f>AVERAGE(G4,H4,I4,J4,F4)</f>
+        <v>4.25</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
       </c>
       <c r="F5" s="2">
         <f>AVERAGE(B5,C5,D5,E5)</f>
-        <v>3.25</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>3.25</v>
+        <v>4</v>
+      </c>
+      <c r="G5" s="7">
+        <v>5</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5</v>
+      </c>
+      <c r="I5" s="7">
+        <v>5</v>
+      </c>
+      <c r="J5" s="7">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <f>AVERAGE(G5,H5,I5,J5,F5)</f>
+        <v>4.2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
       <c r="C6" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
       </c>
       <c r="F6" s="2">
         <f>AVERAGE(B6,C6,D6,E6)</f>
-        <v>4.25</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>3.75</v>
+      </c>
+      <c r="G6" s="7">
+        <v>5</v>
+      </c>
+      <c r="H6" s="7">
+        <v>4</v>
+      </c>
+      <c r="I6" s="7">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3">
+        <f>AVERAGE(G6,H6,I6,J6,F6)</f>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <f>AVERAGE(B7,C7,D7,E7)</f>
+        <v>3.25</v>
+      </c>
+      <c r="G7" s="8">
+        <v>5</v>
+      </c>
+      <c r="H7" s="8">
+        <v>4</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4</v>
+      </c>
+      <c r="J7" s="8">
+        <v>3</v>
+      </c>
+      <c r="K7" s="5">
+        <f>AVERAGE(G7,H7,I7,J7,F7)</f>
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2">
-        <f>AVERAGE(B7,C7,D7,E7)</f>
-        <v>4</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="B8" s="5">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4">
+        <f>AVERAGE(B8,C8,D8,E8)</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="8">
+        <v>4</v>
+      </c>
+      <c r="I8" s="8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="8">
+        <v>3</v>
+      </c>
+      <c r="K8" s="5">
+        <f>AVERAGE(G8,H8,I8,J8,F8)</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4">
+        <f>AVERAGE(B9,C9,D9,E9)</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="8">
+        <v>5</v>
+      </c>
+      <c r="H9" s="8">
+        <v>5</v>
+      </c>
+      <c r="I9" s="8">
+        <v>3</v>
+      </c>
+      <c r="J9" s="8">
+        <v>2</v>
+      </c>
+      <c r="K9" s="5">
+        <f>AVERAGE(G9,H9,I9,J9,F9)</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4">
+        <f>AVERAGE(B10,C10,D10,E10)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="8">
+        <v>4</v>
+      </c>
+      <c r="H10" s="8">
+        <v>4</v>
+      </c>
+      <c r="I10" s="8">
+        <v>4</v>
+      </c>
+      <c r="J10" s="8">
+        <v>3</v>
+      </c>
+      <c r="K10" s="5">
+        <f>AVERAGE(G10,H10,I10,J10,F10)</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5">
+        <v>4</v>
+      </c>
+      <c r="E11" s="5">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4">
+        <f>AVERAGE(B11,C11,D11,E11)</f>
+        <v>3.75</v>
+      </c>
+      <c r="G11" s="8">
+        <v>5</v>
+      </c>
+      <c r="H11" s="8">
+        <v>4</v>
+      </c>
+      <c r="I11" s="8">
+        <v>3</v>
+      </c>
+      <c r="J11" s="8">
+        <v>3</v>
+      </c>
+      <c r="K11" s="5">
+        <f>AVERAGE(G11,H11,I11,J11,F11)</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5">
+        <v>4</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <f>AVERAGE(B12,C12,D12,E12)</f>
+        <v>3.75</v>
+      </c>
+      <c r="G12" s="8">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>4</v>
+      </c>
+      <c r="J12" s="8">
+        <v>2</v>
+      </c>
+      <c r="K12" s="5">
+        <f>AVERAGE(G12,H12,I12,J12,F12)</f>
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <f>AVERAGE(B13,C13,D13,E13)</f>
+        <v>3.25</v>
+      </c>
+      <c r="G13" s="8">
+        <v>5</v>
+      </c>
+      <c r="H13" s="8">
+        <v>4</v>
+      </c>
+      <c r="I13" s="8">
+        <v>3</v>
+      </c>
+      <c r="J13" s="8">
+        <v>2</v>
+      </c>
+      <c r="K13" s="5">
+        <f>AVERAGE(G13,H13,I13,J13,F13)</f>
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2">
-        <f>AVERAGE(B8,C8,D8,E8)</f>
-        <v>3.75</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <f>AVERAGE(B9,C9,D9,E9)</f>
-        <v>3.25</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2">
-        <f>AVERAGE(B10,C10,D10,E10)</f>
-        <v>3.75</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3">
-        <v>2</v>
-      </c>
-      <c r="F11" s="2">
-        <f>AVERAGE(B11,C11,D11,E11)</f>
-        <v>3.25</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3">
-        <v>5</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2">
-        <f>AVERAGE(B12,C12,D12,E12)</f>
-        <v>4.75</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2">
-        <f>AVERAGE(B13,C13,D13,E13)</f>
-        <v>4.25</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>28</v>
-      </c>
-      <c r="B14" s="3">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3">
-        <v>4</v>
-      </c>
-      <c r="E14" s="3">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="B14" s="5">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4">
         <f>AVERAGE(B14,C14,D14,E14)</f>
         <v>3.75</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14">
-        <f t="shared" si="0"/>
+      <c r="G14" s="8">
+        <v>4</v>
+      </c>
+      <c r="H14" s="8">
+        <v>4</v>
+      </c>
+      <c r="I14" s="8">
+        <v>3</v>
+      </c>
+      <c r="J14" s="8">
+        <v>2</v>
+      </c>
+      <c r="K14" s="5">
+        <f>AVERAGE(G14,H14,I14,J14,F14)</f>
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>40</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4">
+        <f>AVERAGE(B15,C15,D15,E15)</f>
         <v>3.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3">
-        <v>4</v>
-      </c>
-      <c r="E15" s="3">
-        <v>3</v>
-      </c>
-      <c r="F15" s="2">
-        <f>AVERAGE(B15,C15,D15,E15)</f>
-        <v>4</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="G15" s="8">
+        <v>5</v>
+      </c>
+      <c r="H15" s="8">
+        <v>3</v>
+      </c>
+      <c r="I15" s="8">
+        <v>3</v>
+      </c>
+      <c r="J15" s="8">
+        <v>2</v>
+      </c>
+      <c r="K15" s="5">
+        <f>AVERAGE(G15,H15,I15,J15,F15)</f>
+        <v>3.35</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>31</v>
-      </c>
-      <c r="B16" s="3">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3">
-        <v>4</v>
-      </c>
-      <c r="D16" s="3">
-        <v>4</v>
-      </c>
-      <c r="E16" s="3">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2</v>
+      </c>
+      <c r="F16" s="4">
         <f>AVERAGE(B16,C16,D16,E16)</f>
-        <v>3.75</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="8">
+        <v>4</v>
+      </c>
+      <c r="H16" s="8">
+        <v>4</v>
+      </c>
+      <c r="I16" s="8">
+        <v>3</v>
+      </c>
+      <c r="J16" s="8">
+        <v>2</v>
+      </c>
+      <c r="K16" s="5">
+        <f>AVERAGE(G16,H16,I16,J16,F16)</f>
+        <v>3.3</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>33</v>
-      </c>
-      <c r="B17" s="3">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3">
-        <v>5</v>
-      </c>
-      <c r="D17" s="3">
-        <v>4</v>
-      </c>
-      <c r="E17" s="3">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="A17" s="4">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3</v>
+      </c>
+      <c r="F17" s="4">
         <f>AVERAGE(B17,C17,D17,E17)</f>
-        <v>4</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.5</v>
+      </c>
+      <c r="G17" s="8">
+        <v>5</v>
+      </c>
+      <c r="H17" s="8">
+        <v>3</v>
+      </c>
+      <c r="I17" s="8">
+        <v>2</v>
+      </c>
+      <c r="J17" s="8">
+        <v>2</v>
+      </c>
+      <c r="K17" s="5">
+        <f>AVERAGE(G17,H17,I17,J17,F17)</f>
+        <v>3.1</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="4">
         <v>36</v>
       </c>
-      <c r="B18" s="3">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="B18" s="5">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4">
         <f>AVERAGE(B18,C18,D18,E18)</f>
         <v>3.25</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>3.25</v>
+      <c r="G18" s="8">
+        <v>3</v>
+      </c>
+      <c r="H18" s="8">
+        <v>3</v>
+      </c>
+      <c r="I18" s="8">
+        <v>3</v>
+      </c>
+      <c r="J18" s="8">
+        <v>3</v>
+      </c>
+      <c r="K18" s="5">
+        <f>AVERAGE(G18,H18,I18,J18,F18)</f>
+        <v>3.05</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>38</v>
-      </c>
-      <c r="B19" s="3">
-        <v>4</v>
-      </c>
-      <c r="C19" s="3">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3">
-        <v>3</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="A19" s="4">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5">
+        <v>4</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4">
         <f>AVERAGE(B19,C19,D19,E19)</f>
         <v>3.5</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
+      <c r="G19" s="8">
+        <v>4</v>
+      </c>
+      <c r="H19" s="8">
+        <v>3</v>
+      </c>
+      <c r="I19" s="8">
+        <v>2</v>
+      </c>
+      <c r="J19" s="8">
+        <v>2</v>
+      </c>
+      <c r="K19" s="5">
+        <f>AVERAGE(G19,H19,I19,J19,F19)</f>
+        <v>2.9</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>40</v>
-      </c>
-      <c r="B20" s="3">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3">
-        <v>3</v>
-      </c>
-      <c r="E20" s="3">
-        <v>3</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="A20" s="4">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5">
+        <v>3</v>
+      </c>
+      <c r="E20" s="5">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4">
         <f>AVERAGE(B20,C20,D20,E20)</f>
-        <v>3.75</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>3.25</v>
+      </c>
+      <c r="G20" s="8">
+        <v>4</v>
+      </c>
+      <c r="H20" s="8">
+        <v>3</v>
+      </c>
+      <c r="I20" s="8">
+        <v>3</v>
+      </c>
+      <c r="J20" s="8">
+        <v>1</v>
+      </c>
+      <c r="K20" s="5">
+        <f>AVERAGE(G20,H20,I20,J20,F20)</f>
+        <v>2.85</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>41</v>
-      </c>
-      <c r="B21" s="3">
-        <v>4</v>
-      </c>
-      <c r="C21" s="3">
-        <v>4</v>
-      </c>
-      <c r="D21" s="3">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3">
-        <v>3</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="A21" s="4">
+        <v>38</v>
+      </c>
+      <c r="B21" s="5">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3</v>
+      </c>
+      <c r="F21" s="4">
         <f>AVERAGE(B21,C21,D21,E21)</f>
         <v>3.5</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21">
+      <c r="G21" s="8">
+        <v>3</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3</v>
+      </c>
+      <c r="I21" s="8">
+        <v>2</v>
+      </c>
+      <c r="J21" s="8">
+        <v>2</v>
+      </c>
+      <c r="K21" s="5">
         <f>AVERAGE(G21,H21,I21,J21,F21)</f>
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K21">
-    <sortCondition ref="A3"/>
+  <sortState ref="A3:K21">
+    <sortCondition descending="1" ref="K2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>